<commit_message>
new chara : durnar, ethan, breeze
</commit_message>
<xml_diff>
--- a/ak-collection-tracker/chara-db.xlsx
+++ b/ak-collection-tracker/chara-db.xlsx
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3122,7 +3122,7 @@
         <v>143</v>
       </c>
       <c r="F95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3202,7 +3202,7 @@
         <v>151</v>
       </c>
       <c r="F99">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3682,7 +3682,7 @@
         <v>201</v>
       </c>
       <c r="F123">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:6">

</xml_diff>